<commit_message>
[UPDATE] Just reviewing code
</commit_message>
<xml_diff>
--- a/generations.xlsx
+++ b/generations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Id</t>
   </si>
@@ -31,34 +31,103 @@
     <t>f(x)</t>
   </si>
   <si>
-    <t>001101</t>
-  </si>
-  <si>
-    <t>101010</t>
-  </si>
-  <si>
-    <t>000100</t>
-  </si>
-  <si>
-    <t>011101</t>
-  </si>
-  <si>
-    <t>14.2884</t>
-  </si>
-  <si>
-    <t>30.4704</t>
-  </si>
-  <si>
-    <t>10.4976</t>
-  </si>
-  <si>
-    <t>22.4676</t>
-  </si>
-  <si>
-    <t>ColA</t>
-  </si>
-  <si>
-    <t>ColB</t>
+    <t>001110</t>
+  </si>
+  <si>
+    <t>001010</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>000110</t>
+  </si>
+  <si>
+    <t>14.7456</t>
+  </si>
+  <si>
+    <t>12.9600</t>
+  </si>
+  <si>
+    <t>24.2064</t>
+  </si>
+  <si>
+    <t>11.2896</t>
+  </si>
+  <si>
+    <t>initial_people</t>
+  </si>
+  <si>
+    <t>max_people</t>
+  </si>
+  <si>
+    <t>variable_a</t>
+  </si>
+  <si>
+    <t>variable_b</t>
+  </si>
+  <si>
+    <t>prob_of_crossing</t>
+  </si>
+  <si>
+    <t>prob_mut_ind</t>
+  </si>
+  <si>
+    <t>prob_mut_gen</t>
+  </si>
+  <si>
+    <t>function_entry</t>
+  </si>
+  <si>
+    <t>delta_x</t>
+  </si>
+  <si>
+    <t>find_x_by</t>
+  </si>
+  <si>
+    <t>iterator_entry</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>jump_numbers</t>
+  </si>
+  <si>
+    <t>points_numbers</t>
+  </si>
+  <si>
+    <t>bits_required</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>0.35</t>
+  </si>
+  <si>
+    <t>x**2</t>
+  </si>
+  <si>
+    <t>Minimización</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t>ColX</t>
@@ -440,13 +509,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,136 +532,198 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2">
-        <v>3.78</v>
+        <v>3.84</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3">
-        <v>5.52</v>
+        <v>3.6</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4">
-        <v>3.24</v>
+        <v>4.92</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5">
-        <v>4.74</v>
+        <v>3.36</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:15">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8">
+        <v>0.06</v>
+      </c>
+      <c r="J8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <v>33.3333</v>
+      </c>
+      <c r="N8">
+        <v>34.3333</v>
+      </c>
+      <c r="O8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="C13" s="1" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="C14" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="C15" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="C16" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIX] Trying to fix
</commit_message>
<xml_diff>
--- a/generations.xlsx
+++ b/generations.xlsx
@@ -14,45 +14,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Id</t>
   </si>
   <si>
-    <t>Numero</t>
-  </si>
-  <si>
-    <t>Binario</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>f(x)</t>
-  </si>
-  <si>
-    <t>110111</t>
-  </si>
-  <si>
-    <t>000110</t>
-  </si>
-  <si>
-    <t>010101</t>
+    <t>Numbers</t>
+  </si>
+  <si>
+    <t>Binary_numbers</t>
+  </si>
+  <si>
+    <t>Values_x</t>
+  </si>
+  <si>
+    <t>Values_f(x)</t>
+  </si>
+  <si>
+    <t>001010</t>
+  </si>
+  <si>
+    <t>101000</t>
+  </si>
+  <si>
+    <t>001101</t>
   </si>
   <si>
     <t>101010</t>
   </si>
   <si>
-    <t>39.6900</t>
-  </si>
-  <si>
-    <t>11.2896</t>
-  </si>
-  <si>
-    <t>18.1476</t>
-  </si>
-  <si>
-    <t>30.4704</t>
+    <t>3.6000</t>
+  </si>
+  <si>
+    <t>5.4000</t>
+  </si>
+  <si>
+    <t>3.7800</t>
+  </si>
+  <si>
+    <t>5.5200</t>
   </si>
   <si>
     <t>initial_people</t>
@@ -67,9 +67,6 @@
     <t>variable_b</t>
   </si>
   <si>
-    <t>prob_of_crossing</t>
-  </si>
-  <si>
     <t>prob_mut_ind</t>
   </si>
   <si>
@@ -112,16 +109,13 @@
     <t>5</t>
   </si>
   <si>
-    <t>0.75</t>
-  </si>
-  <si>
     <t>0.25</t>
   </si>
   <si>
     <t>0.35</t>
   </si>
   <si>
-    <t>x**2</t>
+    <t>x</t>
   </si>
   <si>
     <t>Minimización</t>
@@ -509,13 +503,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,58 +526,58 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:14">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2">
-        <v>6.3</v>
+        <v>3.6</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:14">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3">
-        <v>3.36</v>
+        <v>5.4</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:14">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4">
-        <v>4.26</v>
+        <v>3.78</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:14">
       <c r="A5">
         <v>4</v>
       </c>
@@ -600,7 +594,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -643,87 +637,81 @@
       <c r="N7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>33</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8">
+        <v>0.06</v>
+      </c>
+      <c r="I8" t="s">
         <v>34</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>35</v>
       </c>
-      <c r="I8">
-        <v>0.06</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="K8">
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <v>33.3333</v>
+      </c>
+      <c r="M8">
+        <v>34.3333</v>
+      </c>
+      <c r="N8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="C13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K8" t="s">
+      <c r="D13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L8">
-        <v>2</v>
-      </c>
-      <c r="M8">
-        <v>33.3333</v>
-      </c>
-      <c r="N8">
-        <v>34.3333</v>
-      </c>
-      <c r="O8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="C13" s="1" t="s">
+    </row>
+    <row r="14" spans="1:14">
+      <c r="C14" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="C15" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="C14" t="s">
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="C16" t="s">
         <v>40</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D16" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="C16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>